<commit_message>
Mappings and version 1.0.0
</commit_message>
<xml_diff>
--- a/mappings/ocnbgchem-cmip5-to-cmip6-mappings.xlsx
+++ b/mappings/ocnbgchem-cmip5-to-cmip6-mappings.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
-  <workbookPr date1904="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macg/dev/esdoc/repos/cmip6/cmip6-specializations-ocnbgchem/mappings/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26819"/>
+  <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22700" windowHeight="17540"/>
+    <workbookView xWindow="240" yWindow="100" windowWidth="20740" windowHeight="19140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="91">
   <si>
     <t>Ocean Bio-Geo Chemistry &gt; Tracers &gt; Ecosystem</t>
   </si>
@@ -240,6 +235,66 @@
   </si>
   <si>
     <t>Zooplancton &gt; Type</t>
+  </si>
+  <si>
+    <t>cmip6.ocnbgchem.key_properties.prognostic_variables</t>
+  </si>
+  <si>
+    <t>cmip6.ocnbgchem.key_properties.time_stepping_framework.passive_tracers_transport.method</t>
+  </si>
+  <si>
+    <t>cmip6.ocnbgchem.key_properties.boundary_forcing.atmospheric_deposition</t>
+  </si>
+  <si>
+    <t>cmip6.ocnbgchem.key_properties.boundary_forcing.river_input</t>
+  </si>
+  <si>
+    <t>cmip6.ocnbgchem.key_properties.carbon_chemistry.pH_scale</t>
+  </si>
+  <si>
+    <t>cmip6.ocnbgchem.key_properties.gas_exchange.CO2_exchange_present</t>
+  </si>
+  <si>
+    <t>cmip6.ocnbgchem.key_properties.gas_exchange.O2_exchange_present</t>
+  </si>
+  <si>
+    <t>cmip6.ocnbgchem.key_properties.gas_exchange.O2_exchange_type</t>
+  </si>
+  <si>
+    <t>cmip6.ocnbgchem.key_properties.gas_exchange.CO2_exchange_type</t>
+  </si>
+  <si>
+    <t>cmip6.ocnbgchem.key_properties.gas_exchange.DMS_exchange_present</t>
+  </si>
+  <si>
+    <t>cmip6.ocnbgchem.key_properties.gas_exchange.DMS_exchange_type</t>
+  </si>
+  <si>
+    <t>cmip6.ocnbgchem.key_properties.gas_exchange.N2_exchange_present</t>
+  </si>
+  <si>
+    <t>cmip6.ocnbgchem.key_properties.gas_exchange.N2_exchange_type</t>
+  </si>
+  <si>
+    <t>cmip6.ocnbgchem.key_properties.gas_exchange.N2O_exchange_present</t>
+  </si>
+  <si>
+    <t>cmip6.ocnbgchem.key_properties.gas_exchange.N2O_exchange_type</t>
+  </si>
+  <si>
+    <t>cmip6.ocnbgchem.tracers.sulfur_cycle_present</t>
+  </si>
+  <si>
+    <t>cmip6.ocnbgchem.tracers.particules.method</t>
+  </si>
+  <si>
+    <t>cmip6.ocnbgchem.tracers.ecosystem.phytoplankton.type</t>
+  </si>
+  <si>
+    <t>cmip6.ocnbgchem.tracers.ecosystem.zooplankton.type</t>
+  </si>
+  <si>
+    <t>cmip6.ocnbgchem.tracers.disolved_organic_matter.lability</t>
   </si>
 </sst>
 </file>
@@ -1641,19 +1696,19 @@
   </sheetPr>
   <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A50" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="51.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="84.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="48.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="57.6640625" style="1" customWidth="1"/>
     <col min="4" max="255" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" ht="20.5" customHeight="1">
       <c r="A1" s="12" t="s">
         <v>6</v>
       </c>
@@ -1664,7 +1719,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="20.5" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1673,7 +1728,7 @@
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="20.25" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1682,7 +1737,7 @@
       </c>
       <c r="C3" s="7"/>
     </row>
-    <row r="4" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="20.25" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -1691,7 +1746,7 @@
       </c>
       <c r="C4" s="7"/>
     </row>
-    <row r="5" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" ht="20.25" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
@@ -1700,7 +1755,7 @@
       </c>
       <c r="C5" s="7"/>
     </row>
-    <row r="6" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" ht="20.25" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>1</v>
       </c>
@@ -1709,7 +1764,7 @@
       </c>
       <c r="C6" s="7"/>
     </row>
-    <row r="7" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" ht="20.25" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>1</v>
       </c>
@@ -1718,7 +1773,7 @@
       </c>
       <c r="C7" s="7"/>
     </row>
-    <row r="8" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" ht="20.25" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>1</v>
       </c>
@@ -1727,7 +1782,7 @@
       </c>
       <c r="C8" s="7"/>
     </row>
-    <row r="9" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" ht="20.25" customHeight="1">
       <c r="A9" s="5" t="s">
         <v>1</v>
       </c>
@@ -1736,16 +1791,18 @@
       </c>
       <c r="C9" s="7"/>
     </row>
-    <row r="10" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" ht="20.25" customHeight="1">
       <c r="A10" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="7"/>
-    </row>
-    <row r="11" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C10" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="20.25" customHeight="1">
       <c r="A11" s="5" t="s">
         <v>1</v>
       </c>
@@ -1754,7 +1811,7 @@
       </c>
       <c r="C11" s="7"/>
     </row>
-    <row r="12" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" ht="20.25" customHeight="1">
       <c r="A12" s="5" t="s">
         <v>1</v>
       </c>
@@ -1763,7 +1820,7 @@
       </c>
       <c r="C12" s="7"/>
     </row>
-    <row r="13" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" ht="20.25" customHeight="1">
       <c r="A13" s="5" t="s">
         <v>1</v>
       </c>
@@ -1772,7 +1829,7 @@
       </c>
       <c r="C13" s="7"/>
     </row>
-    <row r="14" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" ht="20.25" customHeight="1">
       <c r="A14" s="5" t="s">
         <v>1</v>
       </c>
@@ -1781,16 +1838,18 @@
       </c>
       <c r="C14" s="7"/>
     </row>
-    <row r="15" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" ht="20.25" customHeight="1">
       <c r="A15" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="7"/>
-    </row>
-    <row r="16" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C15" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="20.25" customHeight="1">
       <c r="A16" s="5" t="s">
         <v>1</v>
       </c>
@@ -1799,7 +1858,7 @@
       </c>
       <c r="C16" s="7"/>
     </row>
-    <row r="17" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" ht="20.25" customHeight="1">
       <c r="A17" s="5" t="s">
         <v>1</v>
       </c>
@@ -1808,7 +1867,7 @@
       </c>
       <c r="C17" s="7"/>
     </row>
-    <row r="18" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" ht="20.25" customHeight="1">
       <c r="A18" s="5" t="s">
         <v>1</v>
       </c>
@@ -1817,30 +1876,34 @@
       </c>
       <c r="C18" s="7"/>
     </row>
-    <row r="19" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" ht="20.25" customHeight="1">
       <c r="A19" s="5"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
     </row>
-    <row r="20" spans="1:3" s="11" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" s="11" customFormat="1" ht="20.25" customHeight="1">
       <c r="A20" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="7"/>
-    </row>
-    <row r="21" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C20" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="20.25" customHeight="1">
       <c r="A21" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="7"/>
-    </row>
-    <row r="22" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C21" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="20.25" customHeight="1">
       <c r="A22" s="5" t="s">
         <v>3</v>
       </c>
@@ -1849,12 +1912,12 @@
       </c>
       <c r="C22" s="7"/>
     </row>
-    <row r="23" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" ht="20.25" customHeight="1">
       <c r="A23" s="5"/>
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
     </row>
-    <row r="24" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" ht="20.25" customHeight="1">
       <c r="A24" s="5" t="s">
         <v>5</v>
       </c>
@@ -1863,7 +1926,7 @@
       </c>
       <c r="C24" s="7"/>
     </row>
-    <row r="25" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" ht="20.25" customHeight="1">
       <c r="A25" s="5" t="s">
         <v>5</v>
       </c>
@@ -1872,7 +1935,7 @@
       </c>
       <c r="C25" s="7"/>
     </row>
-    <row r="26" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" ht="20.25" customHeight="1">
       <c r="A26" s="5" t="s">
         <v>5</v>
       </c>
@@ -1881,16 +1944,18 @@
       </c>
       <c r="C26" s="7"/>
     </row>
-    <row r="27" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3" ht="20.25" customHeight="1">
       <c r="A27" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="7"/>
-    </row>
-    <row r="28" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C27" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="20.25" customHeight="1">
       <c r="A28" s="5" t="s">
         <v>5</v>
       </c>
@@ -1899,7 +1964,7 @@
       </c>
       <c r="C28" s="7"/>
     </row>
-    <row r="29" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3" ht="20.25" customHeight="1">
       <c r="A29" s="5" t="s">
         <v>5</v>
       </c>
@@ -1908,12 +1973,12 @@
       </c>
       <c r="C29" s="7"/>
     </row>
-    <row r="30" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" ht="20.25" customHeight="1">
       <c r="A30" s="5"/>
       <c r="B30" s="6"/>
       <c r="C30" s="7"/>
     </row>
-    <row r="31" spans="1:3" s="11" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" s="11" customFormat="1" ht="20.25" customHeight="1">
       <c r="A31" s="5" t="s">
         <v>4</v>
       </c>
@@ -1922,7 +1987,7 @@
       </c>
       <c r="C31" s="7"/>
     </row>
-    <row r="32" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3" ht="20.25" customHeight="1">
       <c r="A32" s="5" t="s">
         <v>4</v>
       </c>
@@ -1931,79 +1996,95 @@
       </c>
       <c r="C32" s="7"/>
     </row>
-    <row r="33" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" ht="20.25" customHeight="1">
       <c r="A33" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C33" s="7"/>
-    </row>
-    <row r="34" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C33" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="20.25" customHeight="1">
       <c r="A34" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C34" s="7"/>
-    </row>
-    <row r="35" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C34" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="20.25" customHeight="1">
       <c r="A35" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="7"/>
-    </row>
-    <row r="36" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C35" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="20.25" customHeight="1">
       <c r="A36" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="7"/>
-    </row>
-    <row r="37" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C36" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="20.25" customHeight="1">
       <c r="A37" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C37" s="7"/>
-    </row>
-    <row r="38" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C37" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="20.25" customHeight="1">
       <c r="A38" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C38" s="7"/>
-    </row>
-    <row r="39" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C38" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="20.25" customHeight="1">
       <c r="A39" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C39" s="7"/>
-    </row>
-    <row r="40" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C39" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="20.25" customHeight="1">
       <c r="A40" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C40" s="7"/>
-    </row>
-    <row r="41" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C40" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="20.25" customHeight="1">
       <c r="A41" s="5" t="s">
         <v>4</v>
       </c>
@@ -2012,7 +2093,7 @@
       </c>
       <c r="C41" s="7"/>
     </row>
-    <row r="42" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" ht="20.25" customHeight="1">
       <c r="A42" s="5" t="s">
         <v>4</v>
       </c>
@@ -2021,30 +2102,34 @@
       </c>
       <c r="C42" s="7"/>
     </row>
-    <row r="43" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" ht="20.25" customHeight="1">
       <c r="A43" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C43" s="7"/>
-    </row>
-    <row r="44" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C43" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="20.25" customHeight="1">
       <c r="A44" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C44" s="7"/>
-    </row>
-    <row r="45" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C44" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="20.25" customHeight="1">
       <c r="A45" s="5"/>
       <c r="B45" s="6"/>
       <c r="C45" s="7"/>
     </row>
-    <row r="46" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:3" ht="20.25" customHeight="1">
       <c r="A46" s="5" t="s">
         <v>2</v>
       </c>
@@ -2053,7 +2138,7 @@
       </c>
       <c r="C46" s="7"/>
     </row>
-    <row r="47" spans="1:3" s="11" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:3" s="11" customFormat="1" ht="20.25" customHeight="1">
       <c r="A47" s="5" t="s">
         <v>2</v>
       </c>
@@ -2062,16 +2147,18 @@
       </c>
       <c r="C47" s="7"/>
     </row>
-    <row r="48" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:3" ht="20.25" customHeight="1">
       <c r="A48" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C48" s="7"/>
-    </row>
-    <row r="49" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C48" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="20.25" customHeight="1">
       <c r="A49" s="5" t="s">
         <v>2</v>
       </c>
@@ -2080,7 +2167,7 @@
       </c>
       <c r="C49" s="7"/>
     </row>
-    <row r="50" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:3" ht="20.25" customHeight="1">
       <c r="A50" s="5" t="s">
         <v>2</v>
       </c>
@@ -2089,7 +2176,7 @@
       </c>
       <c r="C50" s="7"/>
     </row>
-    <row r="51" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:3" ht="20.25" customHeight="1">
       <c r="A51" s="5" t="s">
         <v>2</v>
       </c>
@@ -2098,7 +2185,7 @@
       </c>
       <c r="C51" s="7"/>
     </row>
-    <row r="52" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:3" ht="20.25" customHeight="1">
       <c r="A52" s="5" t="s">
         <v>2</v>
       </c>
@@ -2107,7 +2194,7 @@
       </c>
       <c r="C52" s="7"/>
     </row>
-    <row r="53" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:3" ht="20.25" customHeight="1">
       <c r="A53" s="5" t="s">
         <v>2</v>
       </c>
@@ -2116,16 +2203,18 @@
       </c>
       <c r="C53" s="7"/>
     </row>
-    <row r="54" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:3" ht="20.25" customHeight="1">
       <c r="A54" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C54" s="7"/>
-    </row>
-    <row r="55" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C54" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="20.25" customHeight="1">
       <c r="A55" s="5" t="s">
         <v>2</v>
       </c>
@@ -2134,7 +2223,7 @@
       </c>
       <c r="C55" s="7"/>
     </row>
-    <row r="56" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:3" ht="20.25" customHeight="1">
       <c r="A56" s="5" t="s">
         <v>2</v>
       </c>
@@ -2143,7 +2232,7 @@
       </c>
       <c r="C56" s="7"/>
     </row>
-    <row r="57" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:3" ht="20.25" customHeight="1">
       <c r="A57" s="5" t="s">
         <v>2</v>
       </c>
@@ -2152,7 +2241,7 @@
       </c>
       <c r="C57" s="7"/>
     </row>
-    <row r="58" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:3" ht="20.25" customHeight="1">
       <c r="A58" s="5" t="s">
         <v>2</v>
       </c>
@@ -2161,21 +2250,23 @@
       </c>
       <c r="C58" s="7"/>
     </row>
-    <row r="59" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:3" ht="20.25" customHeight="1">
       <c r="A59" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C59" s="7"/>
-    </row>
-    <row r="60" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C59" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="20.25" customHeight="1">
       <c r="A60" s="5"/>
       <c r="B60" s="6"/>
       <c r="C60" s="7"/>
     </row>
-    <row r="61" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:3" ht="20.25" customHeight="1">
       <c r="A61" s="5" t="s">
         <v>0</v>
       </c>
@@ -2184,7 +2275,7 @@
       </c>
       <c r="C61" s="7"/>
     </row>
-    <row r="62" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:3" ht="20.25" customHeight="1">
       <c r="A62" s="5" t="s">
         <v>0</v>
       </c>
@@ -2193,7 +2284,7 @@
       </c>
       <c r="C62" s="7"/>
     </row>
-    <row r="63" spans="1:3" s="11" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:3" s="11" customFormat="1" ht="20.25" customHeight="1">
       <c r="A63" s="5" t="s">
         <v>0</v>
       </c>
@@ -2202,7 +2293,7 @@
       </c>
       <c r="C63" s="7"/>
     </row>
-    <row r="64" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:3" ht="20.25" customHeight="1">
       <c r="A64" s="5" t="s">
         <v>0</v>
       </c>
@@ -2211,16 +2302,18 @@
       </c>
       <c r="C64" s="7"/>
     </row>
-    <row r="65" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:3" ht="20.25" customHeight="1">
       <c r="A65" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B65" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C65" s="7"/>
-    </row>
-    <row r="66" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C65" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="20.25" customHeight="1">
       <c r="A66" s="5" t="s">
         <v>0</v>
       </c>
@@ -2229,7 +2322,7 @@
       </c>
       <c r="C66" s="7"/>
     </row>
-    <row r="67" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:3" ht="20.25" customHeight="1">
       <c r="A67" s="5" t="s">
         <v>0</v>
       </c>
@@ -2238,36 +2331,38 @@
       </c>
       <c r="C67" s="7"/>
     </row>
-    <row r="68" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:3" ht="20.25" customHeight="1">
       <c r="A68" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B68" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C68" s="7"/>
-    </row>
-    <row r="69" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C68" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="20.25" customHeight="1">
       <c r="A69" s="8"/>
       <c r="B69" s="9"/>
       <c r="C69" s="10"/>
     </row>
-    <row r="70" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:3" ht="20.25" customHeight="1">
       <c r="A70" s="8"/>
       <c r="B70" s="9"/>
       <c r="C70" s="10"/>
     </row>
-    <row r="71" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:3" ht="20.25" customHeight="1">
       <c r="A71" s="8"/>
       <c r="B71" s="9"/>
       <c r="C71" s="10"/>
     </row>
-    <row r="72" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:3" ht="20.25" customHeight="1">
       <c r="A72" s="8"/>
       <c r="B72" s="9"/>
       <c r="C72" s="10"/>
     </row>
-    <row r="73" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:3" ht="20.25" customHeight="1">
       <c r="A73" s="8"/>
       <c r="B73" s="9"/>
       <c r="C73" s="10"/>
@@ -2282,5 +2377,10 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>